<commit_message>
comment about my bugs
</commit_message>
<xml_diff>
--- a/test/test_android.xlsx
+++ b/test/test_android.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="15200" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="13176" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>未解决</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -44,42 +44,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>绑定不一致的情况，状态是已绑定到人人，但是发布活动时的同步到人人复选框没有打勾的问题。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>先不管。因为之前由于重装app等操作清除掉了app上的人人认证信息，然后又用email登入，这时app上没有人人的认证信息，强行发布也会出错，只好去掉这个复选框，点选时会走人人的认证过程才可能发布。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>算解决</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>app通过人人网登录，程序crash</t>
+  </si>
+  <si>
+    <t>还未能重现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一次使用人人网登录的时候授权页不出现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未能重现。另一方面也不影响发布feed的功能。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>关于(1)
     一方面如果根据假设，不存在这个路径。
     另一方面，如果在 “使用人人号1登录，激活email账号1，登入再解除绑定.为了方便再次使用人人号1通过人人网登入”  的这个时候，假定用户是输入email1得到错误而不得不使用email2的，这时如果对用户使用email 1报错详细一点，
     比如“这个email账号已经存在，你要么用这个email帐号登入后再绑定人人帐号，要么输入一个新的email帐号”，这样的错误信息就应该让用户很清楚该做什么了。
+目前的处理是报了如下的错误信息：“该电子邮件地址已经被使用，如果想把它与当前人人帐号关联，可以用邮件地址登入再在设置中绑定人人帐号”。
   关于(2),根据假设，用户就不用清除数据。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>绑定不一致的情况，状态是已绑定到人人，但是发布活动时的同步到人人复选框没有打勾的问题。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>先不管。因为之前由于重装app等操作清除掉了app上的人人认证信息，然后又用email登入，这时app上没有人人的认证信息，强行发布也会出错，只好去掉这个复选框，点选时会走人人的认证过程才可能发布。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>算解决</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>app通过人人网登录，程序crash</t>
-  </si>
-  <si>
-    <t>还未能重现</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一次使用人人网登录的时候授权页不出现</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,7 +153,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -476,21 +481,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="70.1640625" customWidth="1"/>
-    <col min="3" max="3" width="71.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.19921875" customWidth="1"/>
+    <col min="2" max="2" width="70.19921875" customWidth="1"/>
+    <col min="3" max="3" width="71.296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19">
+    <row r="1" spans="1:3" ht="20.399999999999999">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -501,41 +506,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="170">
+    <row r="2" spans="1:3" ht="226.2">
       <c r="A2" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="68">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="69.599999999999994">
       <c r="A3" s="6"/>
       <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1">
+    </row>
+    <row r="4" spans="1:3" ht="19.95" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>

<commit_message>
added a fixed bug comment
</commit_message>
<xml_diff>
--- a/test/test_android.xlsx
+++ b/test/test_android.xlsx
@@ -59,10 +59,6 @@
     <t>app通过人人网登录，程序crash</t>
   </si>
   <si>
-    <t>还未能重现</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>第一次使用人人网登录的时候授权页不出现</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -77,6 +73,10 @@
     比如“这个email账号已经存在，你要么用这个email帐号登入后再绑定人人帐号，要么输入一个新的email帐号”，这样的错误信息就应该让用户很清楚该做什么了。
 目前的处理是报了如下的错误信息：“该电子邮件地址已经被使用，如果想把它与当前人人帐号关联，可以用邮件地址登入再在设置中绑定人人帐号”。
   关于(2),根据假设，用户就不用清除数据。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>还未能重现。但是umeng那边抓到了错误信息，是“NullPointerException: replacement == null”。已经把这一处修改了。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -104,6 +104,7 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -111,6 +112,7 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -485,14 +487,14 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="1" max="1" width="14.19921875" customWidth="1"/>
     <col min="2" max="2" width="70.19921875" customWidth="1"/>
-    <col min="3" max="3" width="71.296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="71.296875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.399999999999999">
@@ -502,7 +504,7 @@
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -514,7 +516,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="69.599999999999994">
@@ -531,19 +533,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+    </row>
+    <row r="5" spans="1:3" ht="52.2">
       <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -583,6 +585,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added some comments for unclosed bugs
</commit_message>
<xml_diff>
--- a/test/test_android.xlsx
+++ b/test/test_android.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="36540" yWindow="-440" windowWidth="24900" windowHeight="17640" tabRatio="500"/>
+    <workbookView xWindow="36540" yWindow="-444" windowWidth="24900" windowHeight="13176" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>未解决</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -198,15 +198,24 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>拿手机中的message进行测试，test文本在键盘给出的选项中选中后也会出现“输入文字+is saved”的字样，联宇可以作为参考</t>
+    <t>这个是由于网络慢的问题。注册时会发两个api调用，其中第一个是传文本注册信息，第二个是上传photo。第二个会比较慢，失败的概率在网慢的时候较大，从而导致这种情况。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拿手机中的message进行测试，test文本在键盘给出的选项中选中后也会出现“输入文字+is saved”的字样，联宇可以作为参考。
+这么看来，不是我们app的问题了，而是那个htc手机系统本身的问题。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这个目前改不了。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -375,6 +384,33 @@
   </cellXfs>
   <cellStyles count="54">
     <cellStyle name="差" xfId="13" builtinId="27"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -401,33 +437,6 @@
     <cellStyle name="超链接" xfId="48" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="50" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="15" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="17" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="19" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="21" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="23" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="25" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="27" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="29" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="31" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="33" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="35" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="37" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="39" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="41" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -755,21 +764,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="17.399999999999999"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="70.1640625" customWidth="1"/>
-    <col min="3" max="3" width="71.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.19921875" customWidth="1"/>
+    <col min="2" max="2" width="70.19921875" customWidth="1"/>
+    <col min="3" max="3" width="71.296875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19">
+    <row r="1" spans="1:3" ht="20.399999999999999">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -780,7 +789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="221">
+    <row r="2" spans="1:3" ht="226.2">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -791,7 +800,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="68">
+    <row r="3" spans="1:3" ht="69.599999999999994">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -802,7 +811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="68">
+    <row r="4" spans="1:3" ht="69.599999999999994">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -810,7 +819,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1">
+    <row r="5" spans="1:3" ht="19.95" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>27</v>
       </c>
@@ -821,7 +830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="51">
+    <row r="6" spans="1:3" ht="52.2">
       <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
@@ -840,7 +849,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="34">
+    <row r="8" spans="1:3" ht="34.799999999999997">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
@@ -856,7 +865,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="68">
+    <row r="10" spans="1:3" ht="69.599999999999994">
       <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
@@ -864,7 +873,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34">
+    <row r="11" spans="1:3" ht="34.799999999999997">
       <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
@@ -875,7 +884,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34">
+    <row r="12" spans="1:3" ht="34.799999999999997">
       <c r="A12" s="6" t="s">
         <v>27</v>
       </c>
@@ -883,7 +892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="68">
+    <row r="13" spans="1:3" ht="69.599999999999994">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -891,7 +900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="34" customHeight="1">
+    <row r="14" spans="1:3" ht="34.049999999999997" customHeight="1">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -899,7 +908,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34">
+    <row r="15" spans="1:3" ht="34.799999999999997">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -907,7 +916,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="34">
+    <row r="16" spans="1:3" ht="34.799999999999997">
       <c r="A16" s="8" t="s">
         <v>0</v>
       </c>
@@ -915,7 +924,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34">
+    <row r="17" spans="1:3" ht="34.799999999999997">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -923,7 +932,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="34">
+    <row r="18" spans="1:3" ht="34.799999999999997">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -939,15 +948,18 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="51">
+    <row r="20" spans="1:3" ht="52.2">
       <c r="A20" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="34">
+      <c r="C20" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="34.799999999999997">
       <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
@@ -963,13 +975,16 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34">
+    <row r="23" spans="1:3" ht="34.799999999999997">
       <c r="A23" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>35</v>
       </c>
+      <c r="C23" s="4" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="5" t="s">
@@ -987,7 +1002,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34">
+    <row r="26" spans="1:3" ht="34.799999999999997">
       <c r="A26" s="5" t="s">
         <v>15</v>
       </c>
@@ -1003,7 +1018,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="34">
+    <row r="28" spans="1:3" ht="34.799999999999997">
       <c r="A28" s="5" t="s">
         <v>15</v>
       </c>
@@ -1019,7 +1034,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="34">
+    <row r="30" spans="1:3" ht="69.599999999999994">
       <c r="A30" s="8" t="s">
         <v>0</v>
       </c>
@@ -1027,7 +1042,7 @@
         <v>42</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>